<commit_message>
fix date system of pv and net-load original data to everyday(365)
</commit_message>
<xml_diff>
--- a/processed_data/2021_cal_flag.xlsx
+++ b/processed_data/2021_cal_flag.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\yekim\processed_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E9EBF20-D7FE-4EBB-B256-81155DF73E24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BC06257-0D38-4CD8-B377-007CC583507B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26625" yWindow="2025" windowWidth="26580" windowHeight="11385" xr2:uid="{640AA82B-8974-4F9F-9DBA-4D19F3F225DF}"/>
+    <workbookView xWindow="-27495" yWindow="1860" windowWidth="26580" windowHeight="11385" xr2:uid="{640AA82B-8974-4F9F-9DBA-4D19F3F225DF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,9 +36,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>flag</t>
+    <t>date_num</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>load_flag</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -406,14 +410,17 @@
   <dimension ref="A1:C366"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
       <c r="C1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
modify old_load_forecast_model to deal with difference caused by forecast horizon
</commit_message>
<xml_diff>
--- a/processed_data/2021_cal_flag.xlsx
+++ b/processed_data/2021_cal_flag.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\yekim\processed_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0FE257C-9EA6-4248-9846-EB3287154C11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86CAD86C-5EEE-4A74-8038-6E9A9FB98ACB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2220" yWindow="1590" windowWidth="26580" windowHeight="11385" xr2:uid="{640AA82B-8974-4F9F-9DBA-4D19F3F225DF}"/>
+    <workbookView xWindow="630" yWindow="2460" windowWidth="26580" windowHeight="11385" xr2:uid="{640AA82B-8974-4F9F-9DBA-4D19F3F225DF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -440,8 +440,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{333108FB-DE9C-416A-9215-98EEFCFBADDD}">
   <dimension ref="A1:J366"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L333" sqref="L333"/>
+    <sheetView tabSelected="1" topLeftCell="A312" workbookViewId="0">
+      <selection activeCell="J321" sqref="J321"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -9225,13 +9225,13 @@
         <v>321</v>
       </c>
       <c r="C322">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D322">
         <v>0</v>
       </c>
       <c r="E322">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F322">
         <v>1</v>
@@ -9241,6 +9241,9 @@
       </c>
       <c r="H322">
         <v>0</v>
+      </c>
+      <c r="J322">
+        <v>1</v>
       </c>
     </row>
     <row r="323" spans="1:10" x14ac:dyDescent="0.3">

</xml_diff>